<commit_message>
point source functions added
</commit_message>
<xml_diff>
--- a/inst/extdata/pnt_data.xlsx
+++ b/inst/extdata/pnt_data.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Data" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Stations" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -20,12 +21,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="15">
   <si>
     <t xml:space="preserve">name</t>
   </si>
   <si>
-    <t xml:space="preserve">yr</t>
+    <t xml:space="preserve">DATE</t>
   </si>
   <si>
     <t xml:space="preserve">flo</t>
@@ -60,13 +61,20 @@
   <si>
     <t xml:space="preserve">id2</t>
   </si>
+  <si>
+    <t xml:space="preserve">Lat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Long</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -133,12 +141,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -161,16 +173,16 @@
   </sheetPr>
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K30" activeCellId="0" sqref="I30:K35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.54"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -205,12 +217,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="1" t="n">
-        <v>2003</v>
+      <c r="B2" s="2" t="n">
+        <v>37622</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>119.45</v>
@@ -240,12 +252,12 @@
         <v>1.87</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="1" t="n">
-        <v>2004</v>
+      <c r="B3" s="2" t="n">
+        <v>37987</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>106.85</v>
@@ -275,12 +287,12 @@
         <v>0.41</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="1" t="n">
-        <v>2005</v>
+      <c r="B4" s="2" t="n">
+        <v>38353</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>81.64</v>
@@ -310,12 +322,12 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="1" t="n">
-        <v>2006</v>
+      <c r="B5" s="2" t="n">
+        <v>38718</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>116.16</v>
@@ -345,12 +357,12 @@
         <v>3.21</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="1" t="n">
-        <v>2007</v>
+      <c r="B6" s="2" t="n">
+        <v>39083</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>138.36</v>
@@ -380,12 +392,12 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="1" t="n">
-        <v>2008</v>
+      <c r="B7" s="2" t="n">
+        <v>39448</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>166.85</v>
@@ -415,12 +427,12 @@
         <v>2.12</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="1" t="n">
-        <v>2009</v>
+      <c r="B8" s="2" t="n">
+        <v>39814</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>160.55</v>
@@ -450,12 +462,12 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="1" t="n">
-        <v>2010</v>
+      <c r="B9" s="2" t="n">
+        <v>40179</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>197.26</v>
@@ -485,12 +497,12 @@
         <v>1.58</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="1" t="n">
-        <v>2011</v>
+      <c r="B10" s="2" t="n">
+        <v>40544</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>257.53</v>
@@ -520,12 +532,12 @@
         <v>1.78</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="1" t="n">
-        <v>2012</v>
+      <c r="B11" s="2" t="n">
+        <v>40909</v>
       </c>
       <c r="C11" s="1" t="n">
         <v>260.27</v>
@@ -555,12 +567,12 @@
         <v>2.65</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="1" t="n">
-        <v>2013</v>
+      <c r="B12" s="2" t="n">
+        <v>41275</v>
       </c>
       <c r="C12" s="1" t="n">
         <v>271.23</v>
@@ -590,12 +602,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="1" t="n">
-        <v>2014</v>
+      <c r="B13" s="2" t="n">
+        <v>41640</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>279.45</v>
@@ -625,12 +637,12 @@
         <v>1.57</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="1" t="n">
-        <v>2015</v>
+      <c r="B14" s="2" t="n">
+        <v>42005</v>
       </c>
       <c r="C14" s="1" t="n">
         <v>282.19</v>
@@ -660,12 +672,12 @@
         <v>2.72</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="1" t="n">
-        <v>2016</v>
+      <c r="B15" s="2" t="n">
+        <v>42370</v>
       </c>
       <c r="C15" s="1" t="n">
         <v>279.45</v>
@@ -695,12 +707,12 @@
         <v>6.42</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="1" t="n">
-        <v>2017</v>
+      <c r="B16" s="2" t="n">
+        <v>42736</v>
       </c>
       <c r="C16" s="1" t="n">
         <v>271.23</v>
@@ -730,12 +742,12 @@
         <v>2.22</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="1" t="n">
-        <v>2018</v>
+      <c r="B17" s="2" t="n">
+        <v>43101</v>
       </c>
       <c r="C17" s="1" t="n">
         <v>306.85</v>
@@ -765,12 +777,12 @@
         <v>11.36</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="1" t="n">
-        <v>2019</v>
+      <c r="B18" s="2" t="n">
+        <v>43466</v>
       </c>
       <c r="C18" s="1" t="n">
         <v>416.44</v>
@@ -800,12 +812,12 @@
         <v>8.42</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="1" t="n">
-        <v>2020</v>
+      <c r="B19" s="2" t="n">
+        <v>43831</v>
       </c>
       <c r="C19" s="1" t="n">
         <v>391.78</v>
@@ -835,12 +847,12 @@
         <v>8.88</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="1" t="n">
-        <v>2021</v>
+      <c r="B20" s="2" t="n">
+        <v>44197</v>
       </c>
       <c r="C20" s="1" t="n">
         <v>449.32</v>
@@ -870,12 +882,12 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B21" s="1" t="n">
-        <v>2022</v>
+      <c r="B21" s="2" t="n">
+        <v>44562</v>
       </c>
       <c r="C21" s="1" t="n">
         <v>449.32</v>
@@ -905,12 +917,12 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="1" t="n">
-        <v>2003</v>
+      <c r="B22" s="2" t="n">
+        <v>37622</v>
       </c>
       <c r="C22" s="1" t="n">
         <v>19.73</v>
@@ -940,12 +952,12 @@
         <v>3.11</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="1" t="n">
-        <v>2004</v>
+      <c r="B23" s="2" t="n">
+        <v>37987</v>
       </c>
       <c r="C23" s="1" t="n">
         <v>29.59</v>
@@ -975,12 +987,12 @@
         <v>3.11</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="1" t="n">
-        <v>2005</v>
+      <c r="B24" s="2" t="n">
+        <v>38353</v>
       </c>
       <c r="C24" s="1" t="n">
         <v>27.4</v>
@@ -1010,12 +1022,12 @@
         <v>3.11</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="1" t="n">
-        <v>2006</v>
+      <c r="B25" s="2" t="n">
+        <v>38718</v>
       </c>
       <c r="C25" s="1" t="n">
         <v>24.93</v>
@@ -1045,12 +1057,12 @@
         <v>3.11</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="1" t="n">
-        <v>2007</v>
+      <c r="B26" s="2" t="n">
+        <v>39083</v>
       </c>
       <c r="C26" s="1" t="n">
         <v>24.66</v>
@@ -1080,12 +1092,12 @@
         <v>3.11</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B27" s="1" t="n">
-        <v>2008</v>
+      <c r="B27" s="2" t="n">
+        <v>39448</v>
       </c>
       <c r="C27" s="1" t="n">
         <v>24.66</v>
@@ -1115,12 +1127,12 @@
         <v>3.11</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="1" t="n">
-        <v>2009</v>
+      <c r="B28" s="2" t="n">
+        <v>39814</v>
       </c>
       <c r="C28" s="1" t="n">
         <v>50.96</v>
@@ -1150,12 +1162,12 @@
         <v>3.11</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B29" s="1" t="n">
-        <v>2010</v>
+      <c r="B29" s="2" t="n">
+        <v>40179</v>
       </c>
       <c r="C29" s="1" t="n">
         <v>41.1</v>
@@ -1185,12 +1197,12 @@
         <v>3.11</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B30" s="1" t="n">
-        <v>2011</v>
+      <c r="B30" s="2" t="n">
+        <v>40544</v>
       </c>
       <c r="C30" s="1" t="n">
         <v>46.58</v>
@@ -1220,12 +1232,12 @@
         <v>3.11</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B31" s="1" t="n">
-        <v>2012</v>
+      <c r="B31" s="2" t="n">
+        <v>40909</v>
       </c>
       <c r="C31" s="1" t="n">
         <v>41.1</v>
@@ -1255,12 +1267,12 @@
         <v>1.58</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B32" s="1" t="n">
-        <v>2013</v>
+      <c r="B32" s="2" t="n">
+        <v>41275</v>
       </c>
       <c r="C32" s="1" t="n">
         <v>43.84</v>
@@ -1290,12 +1302,12 @@
         <v>1.03</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B33" s="1" t="n">
-        <v>2014</v>
+      <c r="B33" s="2" t="n">
+        <v>41640</v>
       </c>
       <c r="C33" s="1" t="n">
         <v>46.58</v>
@@ -1325,12 +1337,12 @@
         <v>5.38</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B34" s="1" t="n">
-        <v>2015</v>
+      <c r="B34" s="2" t="n">
+        <v>42005</v>
       </c>
       <c r="C34" s="1" t="n">
         <v>63.01</v>
@@ -1360,12 +1372,12 @@
         <v>3.62</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B35" s="1" t="n">
-        <v>2016</v>
+      <c r="B35" s="2" t="n">
+        <v>42370</v>
       </c>
       <c r="C35" s="1" t="n">
         <v>82.19</v>
@@ -1395,12 +1407,12 @@
         <v>20.08</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B36" s="1" t="n">
-        <v>2017</v>
+      <c r="B36" s="2" t="n">
+        <v>42736</v>
       </c>
       <c r="C36" s="1" t="n">
         <v>79.45</v>
@@ -1430,12 +1442,12 @@
         <v>0.87</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B37" s="1" t="n">
-        <v>2018</v>
+      <c r="B37" s="2" t="n">
+        <v>43101</v>
       </c>
       <c r="C37" s="1" t="n">
         <v>84.93</v>
@@ -1465,12 +1477,12 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B38" s="1" t="n">
-        <v>2019</v>
+      <c r="B38" s="2" t="n">
+        <v>43466</v>
       </c>
       <c r="C38" s="1" t="n">
         <v>90.41</v>
@@ -1500,12 +1512,12 @@
         <v>0.68</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B39" s="1" t="n">
-        <v>2020</v>
+      <c r="B39" s="2" t="n">
+        <v>43831</v>
       </c>
       <c r="C39" s="1" t="n">
         <v>84.93</v>
@@ -1535,12 +1547,12 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B40" s="1" t="n">
-        <v>2021</v>
+      <c r="B40" s="2" t="n">
+        <v>44197</v>
       </c>
       <c r="C40" s="1" t="n">
         <v>87.67</v>
@@ -1570,12 +1582,12 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B41" s="1" t="n">
-        <v>2022</v>
+      <c r="B41" s="2" t="n">
+        <v>44562</v>
       </c>
       <c r="C41" s="1" t="n">
         <v>87.67</v>
@@ -1614,4 +1626,64 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="11.53"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>52.62527</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>18.73177</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>52.57165</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>18.62141</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>